<commit_message>
feat(catalogue): renamed provider to institution
</commit_message>
<xml_diff>
--- a/data/datacatalogue/_datacatalogue_schema.xlsx
+++ b/data/datacatalogue/_datacatalogue_schema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/umcg-mswertz/git/molgenis-emx2/data/datacatalogue/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B0AB515-8761-ED44-BA00-C019D96513F2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2D24C6C-534E-6043-AB83-5E0F889676C1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{581C931B-D7B9-8D4C-B6C4-1C49EA2AAD8C}"/>
   </bookViews>
@@ -1720,8 +1720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6827AF39-8A78-C843-9B70-9944F4620E8F}">
   <dimension ref="A1:L234"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="D65" sqref="D65"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2003,7 +2003,7 @@
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
@@ -2822,7 +2822,7 @@
       </c>
       <c r="B45" s="7"/>
       <c r="C45" s="7" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D45" s="8" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
feat: updated catalogue example using OntologyTerms for all the short lookup lists
</commit_message>
<xml_diff>
--- a/data/datacatalogue/_datacatalogue_schema.xlsx
+++ b/data/datacatalogue/_datacatalogue_schema.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/umcg-mswertz/git/molgenis-emx2/data/datacatalogue/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3A4BC70-6829-2B41-8E8B-473857C0AD2C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B59F16E-5585-BF4A-881D-79D6135E02AE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{581C931B-D7B9-8D4C-B6C4-1C49EA2AAD8C}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{581C931B-D7B9-8D4C-B6C4-1C49EA2AAD8C}"/>
   </bookViews>
   <sheets>
     <sheet name="molgenis" sheetId="1" r:id="rId1"/>

</xml_diff>